<commit_message>
Se adjunta Blueprint y documento que define el catálogo de servicios y los atributos de calidad.
</commit_message>
<xml_diff>
--- a/Proyecto I/Actividades de procesos de negocio.xlsx
+++ b/Proyecto I/Actividades de procesos de negocio.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="100" windowWidth="25480" windowHeight="14420" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="25485" windowHeight="14415"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -755,60 +755,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="32.33203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="32.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="6"/>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -816,43 +816,43 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>7</v>
       </c>
@@ -860,37 +860,37 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="1:3" ht="126">
+    <row r="22" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>18</v>
       </c>
@@ -901,7 +901,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>19</v>
       </c>
@@ -912,13 +912,13 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>35</v>
       </c>
@@ -926,31 +926,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="6"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="6"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>7</v>
       </c>
@@ -958,97 +958,97 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B31" s="6"/>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="6"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="6"/>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B37" s="6"/>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B38" s="6"/>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B39" s="6"/>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B40" s="10"/>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B41" s="10"/>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B42" s="10"/>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B43" s="10"/>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B44" s="10"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B45" s="10"/>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>38</v>
       </c>
@@ -1059,25 +1059,25 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B47" s="10"/>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B48" s="10"/>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B49" s="10"/>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>38</v>
       </c>
@@ -1085,67 +1085,67 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B51" s="10"/>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>45</v>
       </c>
       <c r="B52" s="10"/>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B53" s="10"/>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B54" s="10"/>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B55" s="10"/>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B56" s="10"/>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B57" s="10"/>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>51</v>
       </c>
       <c r="B58" s="10"/>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B59" s="10"/>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B60" s="10"/>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>41</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
         <v>55</v>
       </c>
@@ -1161,127 +1161,127 @@
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
         <v>56</v>
       </c>
       <c r="B63" s="12"/>
     </row>
-    <row r="64" spans="1:2" ht="28">
+    <row r="64" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
         <v>57</v>
       </c>
       <c r="B64" s="12"/>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>58</v>
       </c>
       <c r="B65" s="12"/>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>59</v>
       </c>
       <c r="B66" s="12"/>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>60</v>
       </c>
       <c r="B67" s="14"/>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
         <v>61</v>
       </c>
       <c r="B68" s="14"/>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
         <v>62</v>
       </c>
       <c r="B69" s="14"/>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
         <v>63</v>
       </c>
       <c r="B70" s="14"/>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
         <v>64</v>
       </c>
       <c r="B71" s="14"/>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
         <v>65</v>
       </c>
       <c r="B72" s="14"/>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
         <v>66</v>
       </c>
       <c r="B73" s="14"/>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
         <v>67</v>
       </c>
       <c r="B74" s="14"/>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
         <v>68</v>
       </c>
       <c r="B75" s="16"/>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
         <v>69</v>
       </c>
       <c r="B76" s="16"/>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="15" t="s">
         <v>70</v>
       </c>
       <c r="B77" s="16"/>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
         <v>71</v>
       </c>
       <c r="B78" s="16"/>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
         <v>72</v>
       </c>
       <c r="B79" s="16"/>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
         <v>73</v>
       </c>
       <c r="B80" s="16"/>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B81" s="16"/>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
         <v>75</v>
       </c>
       <c r="B82" s="16"/>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="15" t="s">
         <v>76</v>
       </c>
@@ -1302,13 +1302,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="64.83203125" defaultRowHeight="59" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="64.85546875" defaultRowHeight="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="59" customHeight="1" thickBot="1">
+    <row r="1" spans="1:2" ht="59.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="59" customHeight="1" thickBot="1">
+    <row r="2" spans="1:2" ht="59.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -1340,7 +1340,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>